<commit_message>
Update routing resource user
</commit_message>
<xml_diff>
--- a/Struktur_db.xlsx
+++ b/Struktur_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\e-borrow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{328B99EF-933A-4311-A202-908FA6375CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FA72BF-2D4A-44F0-9396-722AA742A07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5A412899-6B4B-4F29-ADCE-B275BBA804D2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>id</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>nama</t>
+  </si>
+  <si>
+    <t>permohonan_id</t>
   </si>
 </sst>
 </file>
@@ -510,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E531675F-6BE0-4126-B706-5B8DCD5EED64}">
-  <dimension ref="B3:H32"/>
+  <dimension ref="B3:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,6 +748,11 @@
         <v>36</v>
       </c>
     </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>